<commit_message>
feat(repository): update project with quieries to fb db
</commit_message>
<xml_diff>
--- a/data/1/МСТиГ/!печать/З/!все группы заочного для печати.xlsx
+++ b/data/1/МСТиГ/!печать/З/!все группы заочного для печати.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwlo\zachetker\data-sharer\data\1\МСТиГ\!печать\З\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EAEF77-14AC-4390-8203-C172A558EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111A0052-46A5-45A4-8B09-6BC6FA0C5E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,14 +23,14 @@
     <sheet name="425" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'411'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'412'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'415'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'416'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'422'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'423'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'425'!$A$3:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'435'!$A$3:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'411'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'412'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'415'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'416'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'422'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'423'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'425'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'435'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="366">
   <si>
     <t>06,09,2023</t>
   </si>
@@ -74,15 +74,6 @@
     <t>№ п/п</t>
   </si>
   <si>
-    <t>Заочное</t>
-  </si>
-  <si>
-    <t>422</t>
-  </si>
-  <si>
-    <t>«Туризм и гостеприимство» второе высшее на 2 курс</t>
-  </si>
-  <si>
     <t>Менеджмент в туризме</t>
   </si>
   <si>
@@ -224,9 +215,6 @@
     <t>Богданик Юлия Витальевна</t>
   </si>
   <si>
-    <t>416</t>
-  </si>
-  <si>
     <t>Менеджмент в спорте</t>
   </si>
   <si>
@@ -410,9 +398,6 @@
     <t>Авласенко Полина Васильевна</t>
   </si>
   <si>
-    <t>415</t>
-  </si>
-  <si>
     <t>Туризм и гостеприимство</t>
   </si>
   <si>
@@ -530,12 +515,6 @@
     <t>Лавицкая Анжелика Александровна</t>
   </si>
   <si>
-    <t>412</t>
-  </si>
-  <si>
-    <t>«Туризм и гостеприимство»</t>
-  </si>
-  <si>
     <t>234182</t>
   </si>
   <si>
@@ -650,9 +629,6 @@
     <t>Алемасова Софья Андреевна</t>
   </si>
   <si>
-    <t>411</t>
-  </si>
-  <si>
     <t>234275</t>
   </si>
   <si>
@@ -773,12 +749,6 @@
     <t>Аврамова Елена Дмитриевна</t>
   </si>
   <si>
-    <t>423</t>
-  </si>
-  <si>
-    <t>«Туризм и гостеприимство» сокращенное на 2 курс</t>
-  </si>
-  <si>
     <t>менеджмент в спорте</t>
   </si>
   <si>
@@ -792,9 +762,6 @@
   </si>
   <si>
     <t>Мякота Алина</t>
-  </si>
-  <si>
-    <t>435</t>
   </si>
   <si>
     <t>08,09,2023</t>
@@ -1179,7 +1146,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1234,14 +1201,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1272,7 +1231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1308,21 +1267,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1348,25 +1298,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1374,12 +1319,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1662,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C3FE5A-BD38-4FA6-9C30-9C416797F34F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1680,62 +1619,91 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -1743,22 +1711,22 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -1766,22 +1734,22 @@
     </row>
     <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -1789,22 +1757,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -1812,22 +1780,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -1835,22 +1803,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -1858,22 +1826,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
@@ -1881,22 +1849,22 @@
     </row>
     <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
@@ -1904,22 +1872,22 @@
     </row>
     <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="F12" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>251</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
@@ -1927,22 +1895,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
@@ -1950,22 +1918,22 @@
     </row>
     <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
@@ -1973,22 +1941,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
@@ -1996,22 +1964,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
@@ -2019,22 +1987,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
@@ -2042,22 +2010,22 @@
     </row>
     <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
@@ -2065,22 +2033,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
@@ -2088,84 +2056,34 @@
     </row>
     <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G22">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2173,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83C6AAE-7382-4E69-9CC8-17B1EE355C9F}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2191,62 +2109,91 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -2254,22 +2201,22 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -2277,22 +2224,22 @@
     </row>
     <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -2300,22 +2247,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -2323,22 +2270,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -2346,22 +2293,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -2369,22 +2316,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
@@ -2392,22 +2339,22 @@
     </row>
     <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
@@ -2415,22 +2362,22 @@
     </row>
     <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
@@ -2438,22 +2385,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
@@ -2461,22 +2408,22 @@
     </row>
     <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
@@ -2484,22 +2431,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
@@ -2507,22 +2454,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
@@ -2530,22 +2477,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
@@ -2553,22 +2500,22 @@
     </row>
     <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>285</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
@@ -2576,22 +2523,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>286</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
@@ -2599,84 +2546,34 @@
     </row>
     <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>289</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G22">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G20">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2684,10 +2581,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CA9F6F-4AB3-430D-B6ED-27D6C837F2E9}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2702,62 +2599,91 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -2765,22 +2691,22 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -2788,22 +2714,22 @@
     </row>
     <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -2811,22 +2737,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -2834,22 +2760,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -2857,22 +2783,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -2880,22 +2806,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
@@ -2903,22 +2829,22 @@
     </row>
     <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
@@ -2926,22 +2852,22 @@
     </row>
     <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
@@ -2949,22 +2875,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
@@ -2972,22 +2898,22 @@
     </row>
     <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
@@ -2995,22 +2921,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
@@ -3018,22 +2944,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
@@ -3041,22 +2967,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
@@ -3064,22 +2990,22 @@
     </row>
     <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
@@ -3087,22 +3013,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
@@ -3110,22 +3036,22 @@
     </row>
     <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
@@ -3133,22 +3059,22 @@
     </row>
     <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
@@ -3156,22 +3082,22 @@
     </row>
     <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
@@ -3179,22 +3105,22 @@
     </row>
     <row r="23" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
@@ -3202,22 +3128,22 @@
     </row>
     <row r="24" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
@@ -3225,22 +3151,22 @@
     </row>
     <row r="25" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
@@ -3248,22 +3174,22 @@
     </row>
     <row r="26" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>0</v>
@@ -3271,22 +3197,22 @@
     </row>
     <row r="27" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>0</v>
@@ -3294,22 +3220,22 @@
     </row>
     <row r="28" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>0</v>
@@ -3317,22 +3243,22 @@
     </row>
     <row r="29" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>0</v>
@@ -3340,22 +3266,22 @@
     </row>
     <row r="30" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>0</v>
@@ -3363,84 +3289,34 @@
     </row>
     <row r="31" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>251</v>
+        <v>57</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>29</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>323</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
-        <v>30</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G33">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3448,10 +3324,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E9E29C-9802-4251-909A-1EAA5980F99B}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3466,61 +3342,91 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="12" t="s">
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>5</v>
+      <c r="E2" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -3528,22 +3434,22 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -3551,22 +3457,22 @@
     </row>
     <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -3574,22 +3480,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -3597,22 +3503,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -3620,22 +3526,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -3643,22 +3549,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
@@ -3666,22 +3572,22 @@
     </row>
     <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
@@ -3689,22 +3595,22 @@
     </row>
     <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
@@ -3712,22 +3618,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>251</v>
+      <c r="E13" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
@@ -3735,22 +3641,22 @@
     </row>
     <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>330</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
@@ -3758,22 +3664,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
@@ -3781,22 +3687,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>332</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
@@ -3804,22 +3710,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>333</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
@@ -3827,22 +3733,22 @@
     </row>
     <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
@@ -3850,22 +3756,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>335</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
@@ -3873,22 +3779,22 @@
     </row>
     <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
@@ -3896,22 +3802,22 @@
     </row>
     <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
@@ -3919,22 +3825,22 @@
     </row>
     <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
@@ -3942,22 +3848,22 @@
     </row>
     <row r="23" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
@@ -3965,83 +3871,34 @@
     </row>
     <row r="24" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>251</v>
+        <v>10</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G26">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4049,10 +3906,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED41D535-846F-44E1-AF8C-7FE2C4CC9DB8}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4067,98 +3924,77 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="E2" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C3" s="5">
         <v>234278</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>366</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="E3" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G5">
-      <sortCondition descending="1" ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G3">
+      <sortCondition descending="1" ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4166,10 +4002,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E562C6-B781-4A41-8606-C2C929CAA8C2}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4184,62 +4020,91 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
@@ -4247,22 +4112,22 @@
     </row>
     <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
@@ -4270,22 +4135,22 @@
     </row>
     <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
@@ -4293,22 +4158,22 @@
     </row>
     <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
@@ -4316,22 +4181,22 @@
     </row>
     <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
@@ -4339,22 +4204,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
@@ -4362,22 +4227,22 @@
     </row>
     <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
@@ -4385,22 +4250,22 @@
     </row>
     <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
@@ -4408,22 +4273,22 @@
     </row>
     <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
@@ -4431,22 +4296,22 @@
     </row>
     <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
@@ -4454,22 +4319,22 @@
     </row>
     <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>354</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
@@ -4477,22 +4342,22 @@
     </row>
     <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
@@ -4500,22 +4365,22 @@
     </row>
     <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>356</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
@@ -4523,22 +4388,22 @@
     </row>
     <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
@@ -4546,22 +4411,22 @@
     </row>
     <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
@@ -4569,22 +4434,22 @@
     </row>
     <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
@@ -4592,22 +4457,22 @@
     </row>
     <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>360</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
@@ -4615,84 +4480,34 @@
     </row>
     <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>361</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>251</v>
+        <v>118</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>240</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>362</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
-        <v>20</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>363</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G23">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4700,10 +4515,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7272DDA9-99B4-42FD-86E0-DD4E29B0AB0E}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4718,121 +4533,102 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="2" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>248</v>
+      <c r="B2" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C4" s="16">
+        <v>204079</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>364</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>365</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
-        <v>367</v>
-      </c>
-      <c r="C7" s="19">
-        <v>204079</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="2">
+        <v>235</v>
+      </c>
+      <c r="E4" s="2">
         <v>813997</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="K14" s="16">
+      <c r="F4" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="K11" s="13">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G23">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4840,10 +4636,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33178DAC-8659-495D-A0D0-59F3CF8F5D1B}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4858,100 +4654,81 @@
     <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8" t="s">
+      <c r="C1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="2" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>373</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="B2" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>375</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="K14" s="16"/>
+      <c r="B3" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="16"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="K12" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G23">
-      <sortCondition ref="C3"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+      <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>